<commit_message>
Implement deterministic in-game channel naming
Replaced random channel generation with a deterministic method based on match ID, cycling through 10 channels (scevo01-scevo10). Updated matchmaking logic, added comprehensive tests, and improved match embed formatting and documentation.
</commit_message>
<xml_diff>
--- a/data/misc/cross_table.xlsx
+++ b/data/misc/cross_table.xlsx
@@ -36,36 +36,16 @@
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
     </style:style>
-    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" style:vertical-align="middle"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0in"/>
-      <style:text-properties fo:font-size="16pt" fo:font-weight="bold" style:font-size-asian="16pt" style:font-weight-asian="bold" style:font-size-complex="16pt" style:font-weight-complex="bold"/>
-    </style:style>
-    <style:style style:name="ce2" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" style:vertical-align="middle"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0in"/>
-      <style:text-properties fo:font-size="12pt" style:font-size-asian="12pt" style:font-size-complex="12pt"/>
-    </style:style>
-    <style:style style:name="ce4" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" style:vertical-align="middle"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0in"/>
-      <style:text-properties fo:font-size="10.5pt" style:font-size-asian="10.5pt" style:font-size-complex="10.5pt"/>
-    </style:style>
-    <style:style style:name="ce5" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" style:vertical-align="middle"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0in"/>
-      <style:text-properties fo:font-size="10.5pt" style:font-size-asian="10.5pt" style:font-size-complex="10.5pt"/>
-    </style:style>
-    <style:style style:name="ce7" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" style:vertical-align="middle"/>
-      <style:paragraph-properties fo:text-align="center" fo:margin-left="0in"/>
-      <style:text-properties fo:font-size="10.5pt" fo:font-weight="bold" style:font-size-asian="10.5pt" style:font-weight-asian="bold" style:font-size-complex="10.5pt" style:font-weight-complex="bold"/>
-    </style:style>
     <style:style style:name="ce11" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" style:vertical-align="middle"/>
       <style:paragraph-properties fo:text-align="center" fo:margin-left="0in"/>
       <style:text-properties fo:font-size="16pt" fo:font-weight="bold" style:font-size-asian="16pt" style:font-weight-asian="bold" style:font-size-complex="16pt" style:font-weight-complex="bold"/>
     </style:style>
+    <style:style style:name="ce15" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" style:vertical-align="middle"/>
+      <style:paragraph-properties fo:text-align="center" fo:margin-left="0in"/>
+      <style:text-properties fo:font-size="10.5pt" fo:font-weight="bold" style:font-size-asian="10.5pt" style:font-weight-asian="bold" style:font-size-complex="10.5pt" style:font-weight-complex="bold"/>
+    </style:style>
     <style:style style:name="ce12" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" style:vertical-align="middle"/>
       <style:paragraph-properties fo:text-align="center" fo:margin-left="0in"/>
@@ -81,10 +61,15 @@
       <style:paragraph-properties fo:text-align="center" fo:margin-left="0in"/>
       <style:text-properties fo:font-size="12pt" style:font-size-asian="12pt" style:font-size-complex="12pt"/>
     </style:style>
-    <style:style style:name="ce15" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce6" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="wrap" style:vertical-align="middle"/>
+      <style:paragraph-properties fo:text-align="center" fo:margin-left="0in"/>
+      <style:text-properties fo:font-size="10.5pt" fo:font-weight="bold" style:font-size-asian="10.5pt" style:font-weight-asian="bold" style:font-size-complex="10.5pt" style:font-weight-complex="bold"/>
+    </style:style>
+    <style:style style:name="ce7" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" style:vertical-align="middle"/>
       <style:paragraph-properties fo:text-align="center" fo:margin-left="0in"/>
-      <style:text-properties fo:font-size="10.5pt" fo:font-weight="bold" style:font-size-asian="10.5pt" style:font-weight-asian="bold" style:font-size-complex="10.5pt" style:font-weight-complex="bold"/>
+      <style:text-properties fo:font-size="10.5pt" fo:font-weight="normal" style:font-size-asian="10.5pt" style:font-weight-asian="normal" style:font-size-complex="10.5pt" style:font-weight-complex="normal"/>
     </style:style>
   </office:automatic-styles>
   <office:body>
@@ -150,65 +135,63 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>NAW</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
             <text:p>US West</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>US Central</text:p>
           </table:table-cell>
+          <table:table-cell table:number-columns-repeated="3" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Korea</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US West</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Korea</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Taiwan</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Korea</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>NAC</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12"/>
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
+            <text:p>US Central</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US Central</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
           <table:table-cell table:number-columns-repeated="2" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>US East</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce12" table:number-columns-repeated="2"/>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US East</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Australia</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Korea</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>NAC</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12"/>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US Central</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US East</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12"/>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US East</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" table:number-columns-repeated="2"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Korea</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12"/>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="5" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US West</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -216,34 +199,27 @@
           </table:table-cell>
           <table:table-cell table:style-name="ce13"/>
           <table:table-cell table:style-name="ce12"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US East</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
-            <text:p>US East</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US East</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>woka</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Korea/US West?</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12"/>
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="3" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="5" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US West</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -252,107 +228,141 @@
           <table:table-cell/>
           <table:table-cell table:style-name="ce12"/>
           <table:table-cell/>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US East</text:p>
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="5" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US West</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>SAM</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" table:number-columns-repeated="4"/>
+          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="3" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US West</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US West</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="5" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US West</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>EUW</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" table:number-columns-repeated="5"/>
+          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+            <text:p>US West</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US West</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="3" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US West</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>EUE</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" table:number-columns-repeated="6"/>
+          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+            <text:p>US West</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US Central</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="3" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US West</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>AFR</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" table:number-columns-repeated="7"/>
+          <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Singapore</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>Singapore</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="3" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Singapore</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>MEA</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="8"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Korea/US West?</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>SAM</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" table:number-columns-repeated="4"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US East</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" table:number-columns-repeated="8"/>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>EUW</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" table:number-columns-repeated="5"/>
-          <table:table-cell table:number-columns-repeated="4" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
-            <text:p>60% US West</text:p>
-            <text:p>40% US Central</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" table:number-columns-repeated="2"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>EUE</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" table:number-columns-repeated="6"/>
-          <table:table-cell table:number-columns-repeated="3" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
-            <text:p>60% US West</text:p>
-            <text:p>40% US Central</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" table:number-columns-repeated="2"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>AFR</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" table:number-columns-repeated="7"/>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
             <text:p>Central EU</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="5" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>Singapore</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Singapore</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>MEA</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" table:number-columns-repeated="8"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="5" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Singapore</text:p>
-          </table:table-cell>
           <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>Central EU</text:p>
           </table:table-cell>
@@ -362,7 +372,7 @@
             <text:p>SEA</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="9"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
             <text:p>Singapore</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="2" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
@@ -384,7 +394,7 @@
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="9"/>
           <table:table-cell/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
             <text:p>Korea</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
@@ -396,7 +406,7 @@
           <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>Singapore</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>Korea</text:p>
           </table:table-cell>
         </table:table-row>
@@ -405,19 +415,19 @@
             <text:p>CHN</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="11"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Korea</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
             <text:p>Taiwan</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Singapore</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
-            <text:p>Singapore</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Taiwan</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Singapore</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
+            <text:p>Singapore</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>Korea</text:p>
           </table:table-cell>
         </table:table-row>
@@ -428,13 +438,13 @@
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="9"/>
           <table:table-cell/>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="2"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
             <text:p>Taiwan</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>Singapore</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>Singapore</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
@@ -446,7 +456,7 @@
             <text:p>OCE</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="13"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
             <text:p>Australia</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
@@ -458,7 +468,10 @@
             <text:p>USB</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="14"/>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>Central EU</text:p>
           </table:table-cell>
         </table:table-row>
@@ -467,7 +480,7 @@
             <text:p>FER</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="15"/>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
             <text:p>Korea</text:p>
           </table:table-cell>
         </table:table-row>
@@ -496,11 +509,11 @@
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.3">
   <office:meta>
     <meta:creation-date>2025-09-13T17:47:57.089000000</meta:creation-date>
-    <dc:date>2025-10-09T21:23:57.362000000</dc:date>
-    <meta:editing-duration>P2DT3H51M29S</meta:editing-duration>
-    <meta:editing-cycles>3</meta:editing-cycles>
+    <dc:date>2025-10-27T18:26:33.208000000</dc:date>
+    <meta:editing-duration>P3DT12H4M33S</meta:editing-duration>
+    <meta:editing-cycles>4</meta:editing-cycles>
     <meta:generator>LibreOffice/24.2.0.3$Windows_X86_64 LibreOffice_project/da48488a73ddd66ea24cf16bbc4f7b9c08e9bea1</meta:generator>
-    <meta:document-statistic meta:table-count="1" meta:cell-count="133" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="1" meta:cell-count="169" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -518,8 +531,8 @@
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">22</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">2</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">13</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">11</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
@@ -575,6 +588,15 @@
       <config:config-item config:name="EmbedFonts" config:type="boolean">false</config:config-item>
       <config:config-item config:name="EmbedLatinScriptFonts" config:type="boolean">true</config:config-item>
       <config:config-item config:name="EmbedOnlyUsedFonts" config:type="boolean">false</config:config-item>
+      <config:config-item-map-indexed config:name="ForbiddenCharacters">
+        <config:config-item-map-entry>
+          <config:config-item config:name="Language" config:type="string">en</config:config-item>
+          <config:config-item config:name="Country" config:type="string">US</config:config-item>
+          <config:config-item config:name="Variant" config:type="string"/>
+          <config:config-item config:name="BeginLine" config:type="string"/>
+          <config:config-item config:name="EndLine" config:type="string"/>
+        </config:config-item-map-entry>
+      </config:config-item-map-indexed>
       <config:config-item config:name="GridColor" config:type="int">12632256</config:config-item>
       <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
       <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
@@ -786,9 +808,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2025-10-12">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2025-10-27">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="23:00:27.845000000">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="15:09:16.322000000">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>

<commit_message>
Add admin tools architecture and advanced scaling docs
Added comprehensive documentation for admin tools architecture and advanced scaling strategies in the docs directory. Updated cross_table.xlsx and removed its lock file. Modified requirements.txt and backend service/database files, and introduced load_monitor.py for backend monitoring.
</commit_message>
<xml_diff>
--- a/data/misc/cross_table.xlsx
+++ b/data/misc/cross_table.xlsx
@@ -136,12 +136,15 @@
             <text:p>NAW</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US Central</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US West, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US Central, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US East, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>US East</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
@@ -151,7 +154,7 @@
             <text:p>Korea</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
+            <text:p>US West, 2</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>Korea</text:p>
@@ -169,24 +172,33 @@
           </table:table-cell>
           <table:table-cell table:style-name="ce12"/>
           <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
-            <text:p>US Central</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US Central</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US East</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
-            <text:p>US East</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>US East</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="5" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US Central, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US Central, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US East, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US East, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US West</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US West, 2</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="3" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>US West</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
@@ -200,21 +212,30 @@
           <table:table-cell table:style-name="ce13"/>
           <table:table-cell table:style-name="ce12"/>
           <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
-            <text:p>US East</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="3" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
-            <text:p>US East</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="5" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US East, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US East, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US East</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US West</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>US West, 2</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="3" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>US West</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
@@ -231,7 +252,10 @@
           <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
             <text:p>US East</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US East, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>US East</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
@@ -256,7 +280,7 @@
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="4"/>
           <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
-            <text:p>US East</text:p>
+            <text:p>US East, 2</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>US East</text:p>
@@ -280,7 +304,7 @@
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="5"/>
           <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
+            <text:p>Central EU, 1</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="2" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>Central EU</text:p>
@@ -289,10 +313,10 @@
             <text:p>Central EU</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
+            <text:p>US West, 4</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US West, 2</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>US West</text:p>
@@ -307,7 +331,7 @@
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="6"/>
           <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
+            <text:p>Central EU, 1</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>Central EU</text:p>
@@ -316,10 +340,10 @@
             <text:p>Central EU</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
-            <text:p>US West</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
-            <text:p>US Central</text:p>
+            <text:p>US West, 4</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>US Central, 3</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="3" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>US West</text:p>
@@ -334,13 +358,13 @@
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="7"/>
           <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Singapore</text:p>
+            <text:p>Central EU, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Singapore, 5</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>Singapore</text:p>
@@ -358,9 +382,12 @@
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="8"/>
           <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="5" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Central EU, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Singapore, 5</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="4" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>Singapore</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
@@ -373,10 +400,13 @@
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="9"/>
           <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
-            <text:p>Singapore</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>Singapore, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>Taiwan</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>Taiwan, 1</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
             <text:p>Singapore</text:p>
@@ -395,40 +425,43 @@
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="9"/>
           <table:table-cell/>
           <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
-            <text:p>Korea</text:p>
+            <text:p>Korea, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Taiwan, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Korea, 1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Singapore, 2</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
+            <text:p>Singapore, 4</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+            <text:p>Korea, 1</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>CHN</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce12" table:number-columns-repeated="11"/>
+          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
+            <text:p>Taiwan, 1</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>Taiwan</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Korea</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Singapore</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
-            <text:p>Korea</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>CHN</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" table:number-columns-repeated="11"/>
-          <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
-            <text:p>Taiwan</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
-            <text:p>Taiwan</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>Singapore</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce7" office:value-type="string" calcext:value-type="string">
             <text:p>Singapore</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
-            <text:p>Korea</text:p>
+            <text:p>Korea, 1</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro1">
@@ -439,7 +472,7 @@
           <table:table-cell/>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="2"/>
           <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
-            <text:p>Taiwan</text:p>
+            <text:p>Taiwan, 1</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>Singapore</text:p>
@@ -457,7 +490,7 @@
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="13"/>
           <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
-            <text:p>Australia</text:p>
+            <text:p>Australia, 1</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="2" table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>Singapore</text:p>
@@ -469,7 +502,7 @@
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="14"/>
           <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
-            <text:p>Central EU</text:p>
+            <text:p>Central EU, 1</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce12" office:value-type="string" calcext:value-type="string">
             <text:p>Central EU</text:p>
@@ -481,7 +514,7 @@
           </table:table-cell>
           <table:table-cell table:style-name="ce12" table:number-columns-repeated="15"/>
           <table:table-cell table:style-name="ce15" office:value-type="string" calcext:value-type="string">
-            <text:p>Korea</text:p>
+            <text:p>Korea, 1</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro2" table:number-rows-repeated="2">
@@ -509,9 +542,9 @@
 <office:document-meta xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" xmlns:ooo="http://openoffice.org/2004/office" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:grddl="http://www.w3.org/2003/g/data-view#" office:version="1.3">
   <office:meta>
     <meta:creation-date>2025-09-13T17:47:57.089000000</meta:creation-date>
-    <dc:date>2025-10-27T18:26:33.208000000</dc:date>
-    <meta:editing-duration>P3DT12H4M33S</meta:editing-duration>
-    <meta:editing-cycles>4</meta:editing-cycles>
+    <dc:date>2025-10-28T10:43:24.611000000</dc:date>
+    <meta:editing-duration>P4DT2H48M41S</meta:editing-duration>
+    <meta:editing-cycles>5</meta:editing-cycles>
     <meta:generator>LibreOffice/24.2.0.3$Windows_X86_64 LibreOffice_project/da48488a73ddd66ea24cf16bbc4f7b9c08e9bea1</meta:generator>
     <meta:document-statistic meta:table-count="1" meta:cell-count="169" meta:object-count="0"/>
   </office:meta>
@@ -531,8 +564,8 @@
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="Sheet1">
-              <config:config-item config:name="CursorPositionX" config:type="int">13</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">11</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">2</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">20</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
@@ -808,7 +841,7 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2025-10-27">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2025-10-28">00/00/0000</text:date>
             , 
             <text:time style:data-style-name="N2" text:time-value="15:09:16.322000000">00:00:00</text:time>
           </text:p>

</xml_diff>